<commit_message>
Mapeo para CU 2.1 Iniciar sesión, y datos para la BD
</commit_message>
<xml_diff>
--- a/Datos/departamento.xlsx
+++ b/Datos/departamento.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HeadHunters\Desktop\Documents\GitHub\proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\GitHub\proyecto\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20405335-A420-4FBD-B3B6-5E994BBE37C2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63183F59-FDC9-4884-BB4F-09150A84C4A4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" xr2:uid="{5BF1BD57-B700-425B-8D51-A8E1E95636F7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Direccion</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>Unidad de Informática</t>
+  </si>
+  <si>
+    <t>iddepartamento</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>idsuperior</t>
   </si>
 </sst>
 </file>
@@ -129,10 +138,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -449,285 +461,299 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F5D410-785D-4141-A6C4-BB831F0C37C7}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1"/>
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
         <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
         <v>2</v>
-      </c>
-      <c r="C3" s="2">
-        <v>3</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2">
         <v>3</v>
-      </c>
-      <c r="C4" s="2">
-        <v>4</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
         <v>4</v>
-      </c>
-      <c r="C5" s="2">
-        <v>5</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2">
         <v>5</v>
-      </c>
-      <c r="C6" s="2">
-        <v>6</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2">
         <v>6</v>
-      </c>
-      <c r="C7" s="2">
-        <v>7</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2">
         <v>7</v>
-      </c>
-      <c r="C8" s="2">
-        <v>8</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2">
         <v>8</v>
-      </c>
-      <c r="C9" s="2">
-        <v>9</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2">
         <v>9</v>
-      </c>
-      <c r="C10" s="2">
-        <v>10</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2">
         <v>10</v>
-      </c>
-      <c r="C11" s="2">
-        <v>11</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2">
         <v>11</v>
-      </c>
-      <c r="C12" s="2">
-        <v>12</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2">
         <v>12</v>
-      </c>
-      <c r="C13" s="2">
-        <v>13</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2">
         <v>13</v>
-      </c>
-      <c r="C14" s="2">
-        <v>14</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2">
         <v>14</v>
-      </c>
-      <c r="C15" s="2">
-        <v>15</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2">
         <v>15</v>
-      </c>
-      <c r="C16" s="2">
-        <v>16</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2">
         <v>16</v>
-      </c>
-      <c r="C17" s="2">
-        <v>17</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2">
         <v>17</v>
-      </c>
-      <c r="C18" s="2">
-        <v>18</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="2">
         <v>18</v>
-      </c>
-      <c r="C19" s="2">
-        <v>19</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="2">
         <v>19</v>
-      </c>
-      <c r="C20" s="2">
-        <v>20</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="2">
         <v>20</v>
-      </c>
-      <c r="C21" s="2">
-        <v>21</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="2">
         <v>21</v>
       </c>
-      <c r="C22" s="2">
-        <v>22</v>
-      </c>
+      <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C24" s="2">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
NoEmpleado ya NO es la llave primaria de Empleado, ahora es idEmpleado
</commit_message>
<xml_diff>
--- a/Datos/departamento.xlsx
+++ b/Datos/departamento.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\GitHub\proyecto\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\parti\proyecto\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63183F59-FDC9-4884-BB4F-09150A84C4A4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560B081B-385E-4BE8-9E72-68C4A50E6F96}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" xr2:uid="{5BF1BD57-B700-425B-8D51-A8E1E95636F7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="31">
   <si>
     <t>Direccion</t>
   </si>
@@ -103,6 +103,21 @@
   </si>
   <si>
     <t>idsuperior</t>
+  </si>
+  <si>
+    <t>permisodocente</t>
+  </si>
+  <si>
+    <t>permisopaee</t>
+  </si>
+  <si>
+    <t>permisodocpaee</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>TRUE</t>
   </si>
 </sst>
 </file>
@@ -138,9 +153,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -461,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F5D410-785D-4141-A6C4-BB831F0C37C7}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,289 +486,484 @@
     <col min="2" max="2" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>2</v>
       </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>3</v>
       </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>4</v>
       </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="D5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>5</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="D6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>6</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="D7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>7</v>
       </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>8</v>
       </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="D9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>9</v>
       </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>10</v>
       </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="D11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>11</v>
       </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="D12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>12</v>
       </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="D13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>13</v>
       </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="D14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>14</v>
       </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="D15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>15</v>
       </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="D16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>16</v>
       </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="D17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>17</v>
       </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="D18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>18</v>
       </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="D19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>19</v>
       </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="D20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>20</v>
       </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="D21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>21</v>
       </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="D22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="D23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>23</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ya coincide el id de tarjeta de perosnal con la RN3
</commit_message>
<xml_diff>
--- a/Datos/departamento.xlsx
+++ b/Datos/departamento.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\parti\proyecto\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\GitHub\iso\proyecto\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560B081B-385E-4BE8-9E72-68C4A50E6F96}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCA924F2-719E-4FFF-9AE2-52B7206EB1C0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" xr2:uid="{5BF1BD57-B700-425B-8D51-A8E1E95636F7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="54">
   <si>
     <t>Direccion</t>
   </si>
@@ -118,6 +118,75 @@
   </si>
   <si>
     <t>TRUE</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
   </si>
 </sst>
 </file>
@@ -478,12 +547,15 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="45.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -507,14 +579,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
+      <c r="A2" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>29</v>
@@ -527,14 +599,14 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
+      <c r="A3" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
-        <v>2</v>
+      <c r="C3" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>29</v>
@@ -547,14 +619,14 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
+      <c r="A4" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
-        <v>3</v>
+      <c r="C4" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>30</v>
@@ -567,14 +639,14 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
+      <c r="A5" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1">
-        <v>4</v>
+      <c r="C5" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>30</v>
@@ -587,14 +659,14 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
+      <c r="A6" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1">
-        <v>5</v>
+      <c r="C6" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>30</v>
@@ -607,14 +679,14 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
+      <c r="A7" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1">
-        <v>6</v>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>30</v>
@@ -627,14 +699,14 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
+      <c r="A8" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1">
-        <v>7</v>
+      <c r="C8" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>29</v>
@@ -647,14 +719,14 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
+      <c r="A9" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1">
-        <v>8</v>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>29</v>
@@ -667,14 +739,14 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
+      <c r="A10" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1">
-        <v>9</v>
+      <c r="C10" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>29</v>
@@ -687,14 +759,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
+      <c r="A11" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1">
-        <v>10</v>
+      <c r="C11" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>29</v>
@@ -707,14 +779,14 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>11</v>
+      <c r="A12" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="1">
-        <v>11</v>
+      <c r="C12" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>30</v>
@@ -727,14 +799,14 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>12</v>
+      <c r="A13" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1">
-        <v>12</v>
+      <c r="C13" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>29</v>
@@ -747,14 +819,14 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>13</v>
+      <c r="A14" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1">
-        <v>13</v>
+      <c r="C14" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>29</v>
@@ -767,14 +839,14 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>14</v>
+      <c r="A15" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="1">
-        <v>14</v>
+      <c r="C15" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>29</v>
@@ -787,14 +859,14 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>15</v>
+      <c r="A16" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="1">
-        <v>15</v>
+      <c r="C16" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>29</v>
@@ -807,14 +879,14 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>16</v>
+      <c r="A17" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="1">
-        <v>16</v>
+      <c r="C17" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>29</v>
@@ -827,14 +899,14 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>17</v>
+      <c r="A18" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="1">
-        <v>17</v>
+      <c r="C18" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>29</v>
@@ -847,14 +919,14 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>18</v>
+      <c r="A19" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="1">
-        <v>18</v>
+      <c r="C19" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>29</v>
@@ -867,14 +939,14 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>19</v>
+      <c r="A20" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="1">
-        <v>19</v>
+      <c r="C20" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>29</v>
@@ -887,14 +959,14 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>20</v>
+      <c r="A21" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="1">
-        <v>20</v>
+      <c r="C21" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>29</v>
@@ -907,14 +979,14 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>21</v>
+      <c r="A22" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="1">
-        <v>21</v>
+      <c r="C22" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>29</v>
@@ -927,14 +999,14 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>22</v>
+      <c r="A23" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="1">
-        <v>22</v>
+      <c r="C23" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>29</v>
@@ -947,14 +1019,14 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>23</v>
+      <c r="A24" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="1">
-        <v>23</v>
+      <c r="C24" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>30</v>

</xml_diff>